<commit_message>
add in dl for shapefiles
</commit_message>
<xml_diff>
--- a/storymap-info/presets.xlsx
+++ b/storymap-info/presets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/escheh/Documents/GitHub/planting.shade/storymap-info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5573A9FA-AB95-C54C-BA10-C91CE156A0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F46A5CA-9CDF-4246-8A4E-E5090DACE706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31260" yWindow="1320" windowWidth="27080" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-65880" yWindow="-1140" windowWidth="50580" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
   <si>
     <t>Variable</t>
   </si>
@@ -116,14 +116,34 @@
       <t xml:space="preserve"> tree canopy had higher priority.</t>
     </r>
   </si>
+  <si>
+    <t>Amount of green space (non-agricultural)</t>
+  </si>
+  <si>
+    <t>Tree canopy coverage in 2021</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -176,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +207,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
@@ -229,9 +255,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -240,56 +266,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:F12"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.1640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -640,9 +729,11 @@
     <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" style="2" customWidth="1"/>
     <col min="3" max="6" width="13.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
@@ -658,8 +749,23 @@
       <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
@@ -669,21 +775,43 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="32"/>
+      <c r="J4" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>5</v>
       </c>
@@ -693,8 +821,17 @@
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+    </row>
+    <row r="6" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
@@ -708,8 +845,17 @@
         <v>8</v>
       </c>
       <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="32"/>
+      <c r="J6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
@@ -721,8 +867,17 @@
         <v>8</v>
       </c>
       <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+    </row>
+    <row r="8" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
@@ -732,8 +887,21 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="32"/>
+      <c r="K8" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
@@ -744,9 +912,24 @@
       <c r="E9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
@@ -760,8 +943,17 @@
       <c r="F10" s="15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="26"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+    </row>
+    <row r="11" spans="2:12" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>15</v>
       </c>
@@ -771,19 +963,36 @@
         <v>8</v>
       </c>
       <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="2:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="20" t="s">
+      <c r="H11" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="38"/>
+    </row>
+    <row r="12" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="H12" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add code for all of mn
</commit_message>
<xml_diff>
--- a/storymap-info/presets.xlsx
+++ b/storymap-info/presets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/escheh/Documents/GitHub/planting.shade/storymap-info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F46A5CA-9CDF-4246-8A4E-E5090DACE706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7811A6F8-CB0B-5445-86B2-869307BD8328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-65880" yWindow="-1140" windowWidth="50580" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1640" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
   <si>
     <t>Variable</t>
   </si>
@@ -127,16 +127,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -255,9 +248,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -266,109 +259,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -377,8 +340,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.1640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -730,7 +711,10 @@
     <col min="2" max="2" width="33.33203125" style="2" customWidth="1"/>
     <col min="3" max="6" width="13.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="12" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -775,19 +759,19 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="H3" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="22"/>
+      <c r="H3" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
@@ -799,17 +783,15 @@
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="32"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
@@ -821,15 +803,15 @@
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="H5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
@@ -845,15 +827,17 @@
         <v>8</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="H6" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
+      <c r="H6" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="28"/>
     </row>
     <row r="7" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
@@ -868,14 +852,18 @@
       </c>
       <c r="F7" s="8"/>
       <c r="H7" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
+        <v>18</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
@@ -887,19 +875,15 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="H8" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="31" t="s">
-        <v>13</v>
-      </c>
+      <c r="H8" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
     </row>
     <row r="9" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
@@ -915,21 +899,17 @@
       <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+    </row>
+    <row r="10" spans="2:12" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
@@ -943,15 +923,15 @@
       <c r="F10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
+      <c r="H10" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
     </row>
     <row r="11" spans="2:12" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
@@ -963,36 +943,27 @@
         <v>8</v>
       </c>
       <c r="F11" s="18"/>
-      <c r="H11" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" s="38"/>
+      <c r="H11" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
     </row>
     <row r="12" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="H12" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>